<commit_message>
added the capacity of the TL
</commit_message>
<xml_diff>
--- a/vhc_matrix_city_excluded.xlsx
+++ b/vhc_matrix_city_excluded.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Surface2\kDrive\SMT\Msc2\Logistic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeliadecaillet/Desktop/MGT-530-SLO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{3F4E79A1-E2A0-4FA1-A826-9A93C6B5D8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B3260E-EC2D-1641-8F6D-931DD0398C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="1" xr2:uid="{9778EEDC-8F73-4A49-985C-AAA669A0840B}"/>
+    <workbookView xWindow="6320" yWindow="2920" windowWidth="21800" windowHeight="13880" xr2:uid="{9778EEDC-8F73-4A49-985C-AAA669A0840B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
   <si>
     <t>Places</t>
   </si>
@@ -329,6 +328,9 @@
   </si>
   <si>
     <t>Riex</t>
+  </si>
+  <si>
+    <t>Bus TL à 2 étages</t>
   </si>
 </sst>
 </file>
@@ -396,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -405,7 +407,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -428,7 +429,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -744,23 +745,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3767D148-2D6C-4BCE-AAA0-AC9E1D736EC5}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.06640625" style="1"/>
-    <col min="3" max="3" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.06640625" style="1"/>
-    <col min="6" max="6" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9" style="1"/>
+    <col min="3" max="3" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -783,7 +784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>16</v>
       </c>
@@ -800,7 +801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>91</v>
       </c>
@@ -813,7 +814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>50</v>
       </c>
@@ -826,7 +827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>20</v>
       </c>
@@ -837,6 +838,19 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>127</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -848,20 +862,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E574F30B-B6FD-48D5-92B2-96351DA13890}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
@@ -871,7 +885,7 @@
       <c r="C1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="6">
+      <c r="D1" s="5">
         <v>18441</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -881,7 +895,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -891,7 +905,7 @@
       <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -901,7 +915,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -921,7 +935,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -941,7 +955,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -959,7 +973,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -976,7 +990,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -993,7 +1007,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1010,7 +1024,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1027,7 +1041,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1044,7 +1058,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1061,7 +1075,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1076,7 +1090,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1087,7 +1101,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1098,7 +1112,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1106,15 +1120,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -1122,7 +1136,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -1130,7 +1144,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -1138,15 +1152,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>66</v>
       </c>
       <c r="B20" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -1154,7 +1168,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1162,67 +1176,67 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B26" s="4" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B27" s="4" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B28" s="4" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B29" s="4" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B30" s="4" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B31" s="4" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B32" s="4" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B33" s="4" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added another TL bus
</commit_message>
<xml_diff>
--- a/vhc_matrix_city_excluded.xlsx
+++ b/vhc_matrix_city_excluded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeliadecaillet/Desktop/MGT-530-SLO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B3260E-EC2D-1641-8F6D-931DD0398C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF31AF77-027B-AF4A-A44A-2C01B3C2F18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6320" yWindow="2920" windowWidth="21800" windowHeight="13880" xr2:uid="{9778EEDC-8F73-4A49-985C-AAA669A0840B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="99">
   <si>
     <t>Places</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>Bus TL à 2 étages</t>
+  </si>
+  <si>
+    <t>Bus Tl à 1 articulation</t>
   </si>
 </sst>
 </file>
@@ -745,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3767D148-2D6C-4BCE-AAA0-AC9E1D736EC5}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -757,7 +760,7 @@
     <col min="3" max="3" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" style="1"/>
     <col min="6" max="6" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -851,6 +854,19 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>